<commit_message>
last step before vacation
</commit_message>
<xml_diff>
--- a/UnempData.xlsx
+++ b/UnempData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="0" windowWidth="20670" windowHeight="9720"/>
+    <workbookView xWindow="7440" yWindow="0" windowWidth="20670" windowHeight="9720"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -353,16 +353,16 @@
     <t>0104</t>
   </si>
   <si>
+    <t>lost_job</t>
+  </si>
+  <si>
+    <t>no_client</t>
+  </si>
+  <si>
+    <t>no_promote</t>
+  </si>
+  <si>
     <t>descriminate</t>
-  </si>
-  <si>
-    <t>lost_job</t>
-  </si>
-  <si>
-    <t>no_client</t>
-  </si>
-  <si>
-    <t>no_promote</t>
   </si>
 </sst>
 </file>
@@ -684,7 +684,7 @@
   <dimension ref="A1:F105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,19 +701,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
drafting dplyr section (mutate and recode is done), next is filter
</commit_message>
<xml_diff>
--- a/UnempData.xlsx
+++ b/UnempData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7440" yWindow="0" windowWidth="20670" windowHeight="9720"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="20670" windowHeight="9720"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,12 +26,15 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="113">
   <si>
-    <t>IDcode</t>
+    <t xml:space="preserve"> recode: any employment discrimination </t>
   </si>
   <si>
     <t>Yes</t>
   </si>
   <si>
+    <t>lost my job</t>
+  </si>
+  <si>
     <t>No</t>
   </si>
   <si>
@@ -41,6 +44,12 @@
     <t>underemployed</t>
   </si>
   <si>
+    <t>removed from direct contact with clients</t>
+  </si>
+  <si>
+    <t xml:space="preserve">denied a promotion </t>
+  </si>
+  <si>
     <t>0001</t>
   </si>
   <si>
@@ -353,16 +362,7 @@
     <t>0104</t>
   </si>
   <si>
-    <t>lost_job</t>
-  </si>
-  <si>
-    <t>no_client</t>
-  </si>
-  <si>
-    <t>no_promote</t>
-  </si>
-  <si>
-    <t>descriminate</t>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -684,113 +684,113 @@
   <dimension ref="A1:F105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>109</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>110</v>
+        <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>111</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>1</v>
@@ -798,99 +798,99 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>1</v>
@@ -898,173 +898,173 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>1</v>
@@ -1073,72 +1073,72 @@
         <v>1</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>1</v>
@@ -1147,278 +1147,278 @@
         <v>1</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>1</v>
@@ -1438,119 +1438,119 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>1</v>
@@ -1558,27 +1558,27 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>1</v>
@@ -1590,7 +1590,7 @@
         <v>1</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>1</v>
@@ -1598,53 +1598,53 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>1</v>
@@ -1653,118 +1653,118 @@
         <v>1</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>1</v>
@@ -1773,12 +1773,12 @@
         <v>1</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>1</v>
@@ -1790,7 +1790,7 @@
         <v>1</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>1</v>
@@ -1798,7 +1798,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>1</v>
@@ -1818,127 +1818,127 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>1</v>
@@ -1947,58 +1947,58 @@
         <v>1</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>1</v>
@@ -2007,24 +2007,24 @@
         <v>1</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>1</v>
@@ -2033,92 +2033,92 @@
         <v>1</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>1</v>
@@ -2127,64 +2127,64 @@
         <v>1</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>1</v>
@@ -2198,67 +2198,67 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>1</v>
@@ -2267,18 +2267,18 @@
         <v>1</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>1</v>
@@ -2290,7 +2290,7 @@
         <v>1</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>1</v>
@@ -2298,13 +2298,13 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>1</v>
@@ -2318,27 +2318,27 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>1</v>
@@ -2350,7 +2350,7 @@
         <v>1</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>1</v>
@@ -2358,227 +2358,227 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>1</v>
@@ -2590,7 +2590,7 @@
         <v>1</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>1</v>
@@ -2598,7 +2598,7 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>1</v>
@@ -2618,7 +2618,7 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>1</v>
@@ -2627,173 +2627,173 @@
         <v>1</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>